<commit_message>
change account to admin, add field gg sheet, gg form to db, fix function complete quarantine for person at tab person and at tab room
</commit_message>
<xml_diff>
--- a/scriptDatabase/fomat_room.xlsx
+++ b/scriptDatabase/fomat_room.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\UIT\Nam 3\HKI\PP OOP\Project\QuanLyKhuCachLy\scriptDatabase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIT\HK5-2020-2021\PhuongPhapPhatTrienPhanMemHuongDoiTuong-SE100.M12\Project\QuanLyKhuCachLy\scriptDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ED0582-6BD4-4DAD-A4C3-91B846688698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{C66F9083-AF61-4625-A103-A6E5C757F8BA}"/>
+    <workbookView xWindow="840" yWindow="-105" windowWidth="22305" windowHeight="13170"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,9 +44,6 @@
     <t>Sức chứa</t>
   </si>
   <si>
-    <t>Loại phòng</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -58,12 +54,15 @@
   </si>
   <si>
     <t>A2</t>
+  </si>
+  <si>
+    <t>Nhóm đối tượng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -414,20 +413,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC2552C-9482-4FD9-96E2-C11F5E73E002}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -438,48 +437,48 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>12</v>

</xml_diff>